<commit_message>
improve servo.c servo.h files
</commit_message>
<xml_diff>
--- a/Ref/电气连接表.xlsx
+++ b/Ref/电气连接表.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\4学习\大二夏\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STM_32_Car\Aks-SmartCar\Aks-SmartCar\Ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCAB9D7-F391-4873-BBF7-CA7BCAE764E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012104C1-8286-494C-9ED1-BED339BBD31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{1220A042-B9C9-4738-A05B-507579105497}"/>
+    <workbookView xWindow="5840" yWindow="2930" windowWidth="19200" windowHeight="11170" xr2:uid="{1220A042-B9C9-4738-A05B-507579105497}"/>
   </bookViews>
   <sheets>
     <sheet name="STM32" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="143">
   <si>
     <t>舵机</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -294,16 +294,6 @@
   <si>
     <t>imu位姿</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PF0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PF1</t>
-  </si>
-  <si>
-    <t>PF2</t>
   </si>
   <si>
     <t>JGB37-520电机编码器1</t>
@@ -586,6 +576,14 @@
   </si>
   <si>
     <t>US3_RX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T2_C1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T2_C2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -676,7 +674,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -725,6 +723,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -755,7 +759,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -828,21 +832,24 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -852,7 +859,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1169,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445FF531-B602-45E7-BB41-083D65F73ADF}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1187,15 +1194,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="7" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -1225,15 +1232,15 @@
         <v>23</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="12" t="s">
@@ -1246,13 +1253,13 @@
         <v>24</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="25"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="12" t="s">
         <v>12</v>
       </c>
@@ -1268,8 +1275,8 @@
       <c r="C5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="25"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28"/>
       <c r="F5" s="12" t="s">
         <v>13</v>
       </c>
@@ -1285,8 +1292,8 @@
       <c r="C6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="25"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="28"/>
       <c r="F6" s="12" t="s">
         <v>43</v>
       </c>
@@ -1302,8 +1309,8 @@
       <c r="C7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="25"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="28"/>
       <c r="F7" s="12" t="s">
         <v>15</v>
       </c>
@@ -1319,8 +1326,8 @@
       <c r="C8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="25"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
       <c r="F8" s="12" t="s">
         <v>16</v>
       </c>
@@ -1331,15 +1338,15 @@
         <v>22</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="28" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="12" t="s">
@@ -1352,13 +1359,13 @@
         <v>25</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="25"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="28"/>
       <c r="F10" s="12" t="s">
         <v>12</v>
       </c>
@@ -1374,8 +1381,8 @@
       <c r="C11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="25"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="28"/>
       <c r="F11" s="12" t="s">
         <v>13</v>
       </c>
@@ -1391,8 +1398,8 @@
       <c r="C12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="25"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="12" t="s">
         <v>14</v>
       </c>
@@ -1408,8 +1415,8 @@
       <c r="C13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="25"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="28"/>
       <c r="F13" s="12" t="s">
         <v>15</v>
       </c>
@@ -1425,8 +1432,8 @@
       <c r="C14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="25"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="28"/>
       <c r="F14" s="12" t="s">
         <v>16</v>
       </c>
@@ -1434,147 +1441,147 @@
     </row>
     <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>70</v>
+      <c r="D15" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>67</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="25"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="28"/>
       <c r="F16" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="25" t="s">
+      <c r="D17" s="27"/>
+      <c r="E17" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="14" t="s">
         <v>71</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>74</v>
       </c>
       <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="25"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="28"/>
       <c r="F18" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="25" t="s">
-        <v>72</v>
+      <c r="D19" s="27"/>
+      <c r="E19" s="28" t="s">
+        <v>69</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="25"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="28"/>
       <c r="F20" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="25" t="s">
-        <v>73</v>
+      <c r="D21" s="27"/>
+      <c r="E21" s="28" t="s">
+        <v>70</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="25"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="28"/>
       <c r="F22" s="15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G22" s="16"/>
     </row>
@@ -1583,15 +1590,15 @@
         <v>50</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="E23" s="28" t="s">
         <v>2</v>
       </c>
       <c r="F23" s="12" t="s">
@@ -1601,16 +1608,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="12" t="s">
         <v>80</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>83</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="26"/>
-      <c r="E24" s="25"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="28"/>
       <c r="F24" s="12" t="s">
         <v>34</v>
       </c>
@@ -1618,16 +1625,16 @@
     </row>
     <row r="25" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="25" t="s">
+      <c r="D25" s="27"/>
+      <c r="E25" s="28" t="s">
         <v>3</v>
       </c>
       <c r="F25" s="12" t="s">
@@ -1637,16 +1644,16 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="25"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="28"/>
       <c r="F26" s="12" t="s">
         <v>34</v>
       </c>
@@ -1657,13 +1664,13 @@
         <v>65</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="26"/>
-      <c r="E27" s="25" t="s">
+      <c r="D27" s="27"/>
+      <c r="E27" s="28" t="s">
         <v>4</v>
       </c>
       <c r="F27" s="12" t="s">
@@ -1673,16 +1680,16 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="26"/>
-      <c r="E28" s="25"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="28"/>
       <c r="F28" s="12" t="s">
         <v>34</v>
       </c>
@@ -1693,21 +1700,21 @@
         <v>54</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="26" t="s">
+      <c r="D29" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="E29" s="28" t="s">
         <v>57</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="G29" s="25" t="s">
+      <c r="G29" s="28" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1716,69 +1723,69 @@
         <v>53</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="26"/>
-      <c r="E30" s="25"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="28"/>
       <c r="F30" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="G30" s="25"/>
+      <c r="G30" s="28"/>
     </row>
     <row r="31" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="26" t="s">
+      <c r="D31" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="25" t="s">
+      <c r="E31" s="28" t="s">
         <v>61</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="G31" s="25" t="s">
+      <c r="G31" s="28" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="26"/>
-      <c r="E32" s="25"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="28"/>
       <c r="F32" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G32" s="25"/>
+      <c r="G32" s="28"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="13" t="s">
-        <v>67</v>
+      <c r="A33" s="33" t="s">
+        <v>103</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>20</v>
+        <v>141</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="D33" s="27" t="s">
         <v>0</v>
       </c>
       <c r="E33" s="18" t="s">
@@ -1790,16 +1797,16 @@
       <c r="G33" s="12"/>
     </row>
     <row r="34" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="13" t="s">
-        <v>68</v>
+      <c r="A34" s="33" t="s">
+        <v>104</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>20</v>
+        <v>142</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="26"/>
+      <c r="D34" s="27"/>
       <c r="E34" s="18" t="s">
         <v>48</v>
       </c>
@@ -1808,47 +1815,37 @@
       </c>
       <c r="G34" s="12"/>
     </row>
-    <row r="35" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="26"/>
-      <c r="E35" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G35" s="12"/>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="8" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="8" t="s">
-        <v>60</v>
-      </c>
+      <c r="A36" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="28"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="28"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="28"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
     </row>
@@ -1861,30 +1858,8 @@
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-    </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A37:E38"/>
-    <mergeCell ref="D3:D8"/>
-    <mergeCell ref="E3:E8"/>
-    <mergeCell ref="D9:D14"/>
-    <mergeCell ref="E9:E14"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D23:D28"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E31:E32"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="G31:G32"/>
     <mergeCell ref="D31:D32"/>
@@ -1894,6 +1869,19 @@
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="D15:D22"/>
     <mergeCell ref="G29:G30"/>
+    <mergeCell ref="A36:E37"/>
+    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="E3:E8"/>
+    <mergeCell ref="D9:D14"/>
+    <mergeCell ref="E9:E14"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D23:D28"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E31:E32"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1922,18 +1910,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>47</v>
@@ -1952,128 +1940,128 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="26">
+      <c r="A3" s="27">
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="27" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="30" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
+        <v>110</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
       <c r="E4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="29"/>
+      <c r="F4" s="30"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="C5" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="27" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="30" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="26"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
+        <v>112</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="29"/>
+      <c r="F6" s="30"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="26">
+      <c r="A7" s="27">
         <v>2</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="C7" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="27" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="30" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
+        <v>110</v>
+      </c>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
       <c r="E8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="29"/>
+      <c r="F8" s="30"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="C9" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="27" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="30" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="26"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
+        <v>112</v>
+      </c>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="29"/>
+      <c r="F10" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -2103,7 +2091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4386C10D-CD79-4639-A4F9-BF9210BFE65A}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -2118,96 +2106,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="A1" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>120</v>
-      </c>
     </row>
     <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
-        <v>141</v>
+      <c r="A3" s="31" t="s">
+        <v>138</v>
       </c>
       <c r="B3" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="31"/>
+      <c r="B4" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="32"/>
+    </row>
+    <row r="5" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="31"/>
+      <c r="B5" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C5" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D5" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="E3" s="31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30"/>
-      <c r="B4" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="31"/>
-    </row>
-    <row r="5" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30"/>
-      <c r="B5" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="32"/>
     </row>
     <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="23" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="12"/>
     </row>
     <row r="7" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.3">
@@ -2216,44 +2204,44 @@
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="22" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="19" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="12"/>
@@ -2264,7 +2252,7 @@
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="19" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="12"/>

</xml_diff>